<commit_message>
MIGENG-65 Added 'Pricing' rules with tests (#6)
* MIGENG-65 Added 'Pricing' rules with tests

* MIGENG-65 Improved the tests after the new fields added to EnvironmentModel
</commit_message>
<xml_diff>
--- a/src/main/resources/org/jboss/xavier/analytics/rules/PricingRule.xlsx
+++ b/src/main/resources/org/jboss/xavier/analytics/rules/PricingRule.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="95">
   <si>
     <t>RuleSet</t>
   </si>
@@ -64,10 +64,7 @@
     <t>environmentModel.sourceProductIndicator == $1</t>
   </si>
   <si>
-    <t>PricingDataModel pricing = new PricingDataModel();</t>
-  </si>
-  <si>
-    <t>pricing.setSourceListValue($1);insert(pricing);</t>
+    <t>PricingDataModel pricing = new PricingDataModel();pricing.setSourceListValue($1);insert(pricing);</t>
   </si>
   <si>
     <t>Which product is the source?</t>
@@ -131,6 +128,174 @@
   </si>
   <si>
     <t>3.5,2.75,2.0</t>
+  </si>
+  <si>
+    <t>RuleTable Vendor Maintenance Price Growth</t>
+  </si>
+  <si>
+    <t>modify(pricing) {setSourceMaintenanceGrowthPercentage($1)}</t>
+  </si>
+  <si>
+    <t>Vendor Maintenance Price Growth</t>
+  </si>
+  <si>
+    <t>Year-over-Year growth in maintenance cost due to breaking ELA</t>
+  </si>
+  <si>
+    <t>RuleTable Switching Costs</t>
+  </si>
+  <si>
+    <t>modify(pricing) {setRhvConsultValue($1)}</t>
+  </si>
+  <si>
+    <t>Switching Costs</t>
+  </si>
+  <si>
+    <t>RHV or RHV Suite Consulting</t>
+  </si>
+  <si>
+    <t>100000.0</t>
+  </si>
+  <si>
+    <t>RuleTable Consulting</t>
+  </si>
+  <si>
+    <t>modify(pricing) {setRhvTAndEValue($1)}</t>
+  </si>
+  <si>
+    <t>Consulting</t>
+  </si>
+  <si>
+    <t>RHV or RHV Suite T&amp;E for consulting</t>
+  </si>
+  <si>
+    <t>30000.0</t>
+  </si>
+  <si>
+    <t>RuleTable Learning</t>
+  </si>
+  <si>
+    <t>modify(pricing) {setRhLearningSubsValue($1)}</t>
+  </si>
+  <si>
+    <t>Learning</t>
+  </si>
+  <si>
+    <t>4 Red Hat Learning subscriptions</t>
+  </si>
+  <si>
+    <t>RuleTable Red Hat Virtualization</t>
+  </si>
+  <si>
+    <t>modify(pricing) {setRhvListValue($1)}</t>
+  </si>
+  <si>
+    <t>modify(pricing) {setRhvDiscountPercentage($1)}</t>
+  </si>
+  <si>
+    <t>List Price</t>
+  </si>
+  <si>
+    <t>Discount</t>
+  </si>
+  <si>
+    <t>Red Hat Virtualization, Premium</t>
+  </si>
+  <si>
+    <t>1500.0</t>
+  </si>
+  <si>
+    <t>RuleTable Red Hat CloudForms</t>
+  </si>
+  <si>
+    <t>modify(pricing) {setRhCFListValue($1)}</t>
+  </si>
+  <si>
+    <t>modify(pricing) {setRhCFDiscountPercentage($1)}</t>
+  </si>
+  <si>
+    <t>Red Hat CloudForms, Premium</t>
+  </si>
+  <si>
+    <t>2400.0</t>
+  </si>
+  <si>
+    <t>RuleTable Red Hat OpenShift</t>
+  </si>
+  <si>
+    <t>modify(pricing) {setRhOSListValue($1)}</t>
+  </si>
+  <si>
+    <t>modify(pricing) {setRhOSDiscountPercentage($1)}</t>
+  </si>
+  <si>
+    <t>Red Hat OpenShift, Premium</t>
+  </si>
+  <si>
+    <t>15000.0</t>
+  </si>
+  <si>
+    <t>0.0</t>
+  </si>
+  <si>
+    <t>RuleTable Red Hat Virtualization Suite</t>
+  </si>
+  <si>
+    <t>modify(pricing) {setRhVirtListValue($1)}</t>
+  </si>
+  <si>
+    <t>modify(pricing) {setRhVirtDiscountPercentage($1)}</t>
+  </si>
+  <si>
+    <t>Red Hat Virtualization Suite, Premium</t>
+  </si>
+  <si>
+    <t>2800.0</t>
+  </si>
+  <si>
+    <t>RuleTable Free Red Hat subscriptions</t>
+  </si>
+  <si>
+    <t>modify(pricing) {setFreeSubsYear1Indicator($1),setFreeSubsYear2And3Indicator($2);}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1st year, 2nd&amp;3rd year </t>
+  </si>
+  <si>
+    <t>Free Red Hat subscriptions</t>
+  </si>
+  <si>
+    <t>true, false</t>
+  </si>
+  <si>
+    <t>RuleTable Red Hat Pricing Effective</t>
+  </si>
+  <si>
+    <t>environmentModel.dealIndicator == $1</t>
+  </si>
+  <si>
+    <t>modify(pricing) {setRhvValue(pricing.getRhvDiscountPercentage() - $1)}</t>
+  </si>
+  <si>
+    <t>modify(pricing) {setRhCFValue(pricing.getRhCFDiscountPercentage() - $1)}</t>
+  </si>
+  <si>
+    <t>modify(pricing) {setRhOSValue(pricing.getRhOSDiscountPercentage() - $1)}</t>
+  </si>
+  <si>
+    <t>modify(pricing) {setRhVirtValue(pricing.getRhVirtDiscountPercentage() - $1)}</t>
+  </si>
+  <si>
+    <t>Red Hat Pricing Effective</t>
+  </si>
+  <si>
+    <t>0.1</t>
+  </si>
+  <si>
+    <t>0.2</t>
+  </si>
+  <si>
+    <t>0.3</t>
   </si>
 </sst>
 </file>
@@ -187,7 +352,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -222,32 +387,35 @@
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
     <xf borderId="0" fillId="4" fontId="1" numFmtId="10" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="10" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -271,20 +439,19 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="40.71"/>
-    <col customWidth="1" min="2" max="2" width="32.29"/>
-    <col customWidth="1" min="3" max="3" width="54.14"/>
-    <col customWidth="1" min="4" max="4" width="46.86"/>
-    <col customWidth="1" min="5" max="5" width="34.71"/>
-    <col customWidth="1" min="6" max="6" width="28.71"/>
-    <col customWidth="1" min="7" max="7" width="20.71"/>
+    <col customWidth="1" min="1" max="1" width="54.14"/>
+    <col customWidth="1" hidden="1" min="2" max="2" width="41.29"/>
+    <col customWidth="1" min="3" max="3" width="39.57"/>
+    <col customWidth="1" min="4" max="4" width="15.71"/>
+    <col customWidth="1" min="5" max="6" width="37.0"/>
+    <col customWidth="1" min="7" max="7" width="63.86"/>
     <col customWidth="1" min="8" max="8" width="25.57"/>
     <col customWidth="1" min="9" max="9" width="23.71"/>
     <col customWidth="1" min="10" max="10" width="12.29"/>
     <col customWidth="1" min="11" max="12" width="73.29"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" hidden="1">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -293,7 +460,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" hidden="1">
       <c r="A2" s="3"/>
       <c r="B2" s="4" t="s">
         <v>2</v>
@@ -324,7 +491,7 @@
       <c r="Y2" s="3"/>
       <c r="Z2" s="3"/>
     </row>
-    <row r="3">
+    <row r="3" hidden="1">
       <c r="B3" s="4" t="s">
         <v>2</v>
       </c>
@@ -332,7 +499,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" hidden="1">
       <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
@@ -340,7 +507,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" ht="16.5" customHeight="1">
+    <row r="5" ht="16.5" hidden="1" customHeight="1">
       <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
@@ -348,7 +515,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7">
+    <row r="6" hidden="1"/>
+    <row r="7" hidden="1">
       <c r="A7" s="7" t="s">
         <v>8</v>
       </c>
@@ -369,12 +537,12 @@
     <row r="10">
       <c r="B10" s="1"/>
     </row>
-    <row r="11">
+    <row r="11" hidden="1">
       <c r="B11" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" hidden="1">
       <c r="A12" s="2" t="s">
         <v>12</v>
       </c>
@@ -384,9 +552,7 @@
       <c r="C12" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>14</v>
-      </c>
+      <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="10"/>
       <c r="G12" s="10"/>
@@ -396,28 +562,25 @@
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
     </row>
-    <row r="13">
+    <row r="13" hidden="1">
       <c r="B13" s="2" t="s">
         <v>15</v>
       </c>
       <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
     </row>
-    <row r="14">
+    <row r="14" hidden="1">
       <c r="B14" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D14" s="12" t="s">
-        <v>18</v>
-      </c>
+      <c r="D14" s="12"/>
       <c r="E14" s="1"/>
       <c r="F14" s="13"/>
       <c r="G14" s="13"/>
@@ -429,14 +592,12 @@
     </row>
     <row r="15">
       <c r="B15" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>20</v>
-      </c>
+      <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
@@ -447,17 +608,15 @@
     </row>
     <row r="16">
       <c r="A16" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B16" s="9">
         <v>1.0</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="D16" s="14" t="s">
-        <v>22</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="D16" s="15"/>
       <c r="E16" s="15"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
@@ -469,17 +628,15 @@
     </row>
     <row r="17">
       <c r="A17" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B17" s="9">
         <v>2.0</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="D17" s="14" t="s">
-        <v>24</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="D17" s="15"/>
       <c r="E17" s="15"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
@@ -489,12 +646,12 @@
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
     </row>
-    <row r="19">
+    <row r="19" hidden="1">
       <c r="B19" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="20">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" hidden="1">
       <c r="A20" s="2" t="s">
         <v>12</v>
       </c>
@@ -508,46 +665,46 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" hidden="1">
       <c r="B21" s="16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C21" s="11"/>
       <c r="D21" s="2"/>
     </row>
-    <row r="22">
+    <row r="22" hidden="1">
       <c r="B22" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="D22" s="17" t="s">
         <v>28</v>
-      </c>
-      <c r="D22" s="12" t="s">
-        <v>29</v>
       </c>
       <c r="E22" s="1"/>
     </row>
     <row r="23">
       <c r="B23" s="1"/>
       <c r="C23" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D23" s="8" t="s">
         <v>30</v>
-      </c>
-      <c r="D23" s="8" t="s">
-        <v>31</v>
       </c>
       <c r="E23" s="1"/>
     </row>
     <row r="24">
       <c r="A24" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B24" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C24" s="17">
+      <c r="C24" s="18">
         <v>0.1</v>
       </c>
-      <c r="D24" s="17">
+      <c r="D24" s="18">
         <v>0.75</v>
       </c>
       <c r="E24" s="15"/>
@@ -556,12 +713,12 @@
       <c r="B25" s="1"/>
       <c r="E25" s="15"/>
     </row>
-    <row r="26">
+    <row r="26" hidden="1">
       <c r="B26" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="27">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="27" hidden="1">
       <c r="A27" s="2" t="s">
         <v>12</v>
       </c>
@@ -573,65 +730,89 @@
       </c>
       <c r="E27" s="1"/>
     </row>
-    <row r="28">
+    <row r="28" hidden="1">
       <c r="B28" s="16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C28" s="11"/>
     </row>
-    <row r="29">
+    <row r="29" hidden="1">
       <c r="B29" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C29" s="17" t="s">
         <v>35</v>
-      </c>
-      <c r="C29" s="12" t="s">
-        <v>36</v>
       </c>
       <c r="E29" s="1"/>
     </row>
     <row r="30">
       <c r="B30" s="1"/>
       <c r="C30" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E30" s="1"/>
     </row>
     <row r="31">
       <c r="A31" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C31" s="14" t="s">
         <v>38</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C31" s="14" t="s">
-        <v>39</v>
       </c>
       <c r="E31" s="15"/>
     </row>
     <row r="32">
       <c r="B32" s="1"/>
     </row>
-    <row r="33">
-      <c r="B33" s="1"/>
-    </row>
-    <row r="34">
-      <c r="A34" s="1"/>
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
-    </row>
-    <row r="35">
-      <c r="B35" s="18"/>
-    </row>
-    <row r="36">
-      <c r="B36" s="1"/>
-      <c r="C36" s="19"/>
+    <row r="33" hidden="1">
+      <c r="B33" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="34" hidden="1">
+      <c r="A34" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="35" hidden="1">
+      <c r="B35" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C35" s="11"/>
+    </row>
+    <row r="36" hidden="1">
+      <c r="B36" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C36" s="17" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="37">
-      <c r="C37" s="1"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="8" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="38">
-      <c r="A38" s="1"/>
-      <c r="B38" s="1"/>
-      <c r="C38" s="15"/>
+      <c r="A38" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C38" s="18">
+        <v>0.15</v>
+      </c>
       <c r="E38" s="10"/>
       <c r="F38" s="10"/>
       <c r="G38" s="10"/>
@@ -639,41 +820,48 @@
       <c r="I38" s="10"/>
     </row>
     <row r="39">
-      <c r="B39" s="20"/>
+      <c r="B39" s="19"/>
       <c r="E39" s="3"/>
       <c r="F39" s="3"/>
       <c r="G39" s="3"/>
       <c r="H39" s="3"/>
       <c r="I39" s="3"/>
     </row>
-    <row r="40">
-      <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
-      <c r="D40" s="1"/>
-      <c r="E40" s="13"/>
-      <c r="F40" s="13"/>
-      <c r="G40" s="13"/>
-      <c r="H40" s="13"/>
-      <c r="I40" s="13"/>
-      <c r="J40" s="1"/>
-      <c r="K40" s="1"/>
-      <c r="L40" s="1"/>
-    </row>
-    <row r="41">
-      <c r="B41" s="1"/>
-      <c r="C41" s="1"/>
+    <row r="40" hidden="1">
+      <c r="B40" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="3"/>
+      <c r="H40" s="3"/>
+      <c r="I40" s="3"/>
+    </row>
+    <row r="41" hidden="1">
+      <c r="A41" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D41" s="1"/>
-      <c r="E41" s="1"/>
-      <c r="F41" s="1"/>
-      <c r="G41" s="1"/>
-      <c r="H41" s="1"/>
-      <c r="I41" s="1"/>
+      <c r="E41" s="13"/>
+      <c r="F41" s="13"/>
+      <c r="G41" s="13"/>
+      <c r="H41" s="13"/>
+      <c r="I41" s="13"/>
       <c r="J41" s="1"/>
-    </row>
-    <row r="42">
-      <c r="A42" s="1"/>
-      <c r="B42" s="1"/>
-      <c r="C42" s="1"/>
+      <c r="K41" s="1"/>
+      <c r="L41" s="1"/>
+    </row>
+    <row r="42" hidden="1">
+      <c r="B42" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C42" s="11"/>
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
@@ -681,8 +869,552 @@
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
       <c r="J42" s="1"/>
-      <c r="K42" s="1"/>
-      <c r="L42" s="1"/>
+    </row>
+    <row r="43" hidden="1">
+      <c r="B43" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C43" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
+      <c r="F43" s="1"/>
+      <c r="G43" s="1"/>
+      <c r="H43" s="1"/>
+      <c r="I43" s="1"/>
+      <c r="J43" s="1"/>
+      <c r="K43" s="1"/>
+      <c r="L43" s="1"/>
+    </row>
+    <row r="44">
+      <c r="B44" s="1"/>
+      <c r="C44" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C45" s="14" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="46" hidden="1"/>
+    <row r="47" hidden="1">
+      <c r="B47" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="48" hidden="1">
+      <c r="A48" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="49" hidden="1">
+      <c r="B49" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C49" s="11"/>
+    </row>
+    <row r="50" hidden="1">
+      <c r="B50" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C50" s="17" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="B51" s="1"/>
+      <c r="C51" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C52" s="14" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="53" hidden="1"/>
+    <row r="54" hidden="1">
+      <c r="B54" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="55" hidden="1">
+      <c r="A55" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="56" hidden="1">
+      <c r="B56" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C56" s="11"/>
+    </row>
+    <row r="57" hidden="1">
+      <c r="B57" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C57" s="17" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="B58" s="1"/>
+      <c r="C58" s="8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C59" s="14" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="61" hidden="1">
+      <c r="B61" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="62" hidden="1">
+      <c r="A62" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="63" hidden="1">
+      <c r="B63" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C63" s="11"/>
+      <c r="D63" s="11"/>
+    </row>
+    <row r="64" hidden="1">
+      <c r="B64" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C64" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="D64" s="17" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="B65" s="1"/>
+      <c r="C65" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="D65" s="8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C66" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="D66" s="18">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="67" hidden="1"/>
+    <row r="68" hidden="1">
+      <c r="B68" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="69" hidden="1">
+      <c r="A69" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="70" hidden="1">
+      <c r="B70" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C70" s="11"/>
+      <c r="D70" s="11"/>
+    </row>
+    <row r="71" hidden="1">
+      <c r="B71" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C71" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="D71" s="17" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="B72" s="1"/>
+      <c r="C72" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="D72" s="8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C73" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="D73" s="18">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="74" hidden="1"/>
+    <row r="75" hidden="1">
+      <c r="B75" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="76" hidden="1">
+      <c r="A76" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="77" hidden="1">
+      <c r="B77" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C77" s="11"/>
+      <c r="D77" s="11"/>
+    </row>
+    <row r="78" hidden="1">
+      <c r="B78" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C78" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="D78" s="17" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="B79" s="1"/>
+      <c r="C79" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="D79" s="8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C80" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="D80" s="14" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="81" hidden="1"/>
+    <row r="82" hidden="1">
+      <c r="B82" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="83" hidden="1">
+      <c r="A83" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D83" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="84" hidden="1">
+      <c r="B84" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C84" s="11"/>
+      <c r="D84" s="11"/>
+    </row>
+    <row r="85" hidden="1">
+      <c r="B85" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C85" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="D85" s="17" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="B86" s="1"/>
+      <c r="C86" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="D86" s="8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C87" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="D87" s="18">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="89" hidden="1">
+      <c r="B89" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="90" hidden="1">
+      <c r="A90" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D90" s="1"/>
+    </row>
+    <row r="91" hidden="1">
+      <c r="B91" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C91" s="11"/>
+    </row>
+    <row r="92" hidden="1">
+      <c r="B92" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C92" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="D92" s="12"/>
+    </row>
+    <row r="93">
+      <c r="B93" s="1"/>
+      <c r="C93" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="D93" s="1"/>
+    </row>
+    <row r="94">
+      <c r="A94" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C94" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="D94" s="20"/>
+    </row>
+    <row r="96" hidden="1">
+      <c r="B96" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="97" hidden="1">
+      <c r="A97" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C97" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D97" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E97" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F97" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G97" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="98" hidden="1">
+      <c r="B98" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C98" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D98" s="11"/>
+      <c r="E98" s="11"/>
+      <c r="F98" s="11"/>
+      <c r="G98" s="11"/>
+    </row>
+    <row r="99" hidden="1">
+      <c r="B99" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C99" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D99" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="E99" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="F99" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="G99" s="17" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="100" hidden="1">
+      <c r="B100" s="1"/>
+      <c r="C100" s="1"/>
+      <c r="D100" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E100" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F100" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="G100" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="101" hidden="1">
+      <c r="A101" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C101" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="D101" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="E101" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="F101" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="G101" s="21" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="102" hidden="1">
+      <c r="A102" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C102" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="D102" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="E102" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="F102" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="G102" s="21" t="s">
+        <v>92</v>
+      </c>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>